<commit_message>
tracking updates and creating additional email protocol templates as necessary
</commit_message>
<xml_diff>
--- a/documents/protocol_and_emails/organizationSheet.xlsx
+++ b/documents/protocol_and_emails/organizationSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EyegazeTrackerPINEntry\documents\protocol_and_emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CAA5C2-8F05-4F65-AE28-45A6ECFA02FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6896333F-0E33-488D-A2A0-12619CAFEE97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Participant ID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>"0001"</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>Tobii Dynavox I-13</t>
   </si>
   <si>
@@ -87,10 +84,49 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Gift card sent</t>
-  </si>
-  <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>tobii dynaoxs</t>
+  </si>
+  <si>
+    <t>Grid 3 computer control </t>
+  </si>
+  <si>
+    <t> PCEye Plus from TobiiDynavox</t>
+  </si>
+  <si>
+    <t>Windows Eye Control</t>
+  </si>
+  <si>
+    <t>PCEye 5</t>
+  </si>
+  <si>
+    <t>Tobii Dynavox Computer Control</t>
+  </si>
+  <si>
+    <t>Tobii 4C</t>
+  </si>
+  <si>
+    <t>Grid 3</t>
+  </si>
+  <si>
+    <t>Owns multiple eye gaze trackers, was told to choose one that was most comfortable, still need confirmation of what the study was completed with</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>Gift card form sent</t>
+  </si>
+  <si>
+    <t>Gift card confirmed</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -133,11 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K202"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,9 +468,10 @@
     <col min="5" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,10 +482,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -458,19 +494,22 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -478,26 +517,26 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>1006</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
         <v>44316</v>
       </c>
       <c r="F3" s="1">
@@ -509,104 +548,185 @@
       <c r="H3" s="1">
         <v>44320</v>
       </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I3" s="1">
+        <v>44323</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1087</v>
       </c>
-      <c r="E4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1">
         <v>44315</v>
       </c>
       <c r="F4" s="1">
         <v>44316</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <v>44334</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44334</v>
+      </c>
+      <c r="I4" s="1">
+        <v>44335</v>
+      </c>
+      <c r="K4" s="1">
+        <v>44334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1249</v>
       </c>
-      <c r="E5" s="3">
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1">
         <v>44315</v>
       </c>
       <c r="F5" s="1">
         <v>44316</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G5" s="1">
+        <v>44335</v>
+      </c>
+      <c r="K5" s="1">
+        <v>44334</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>1298</v>
       </c>
-      <c r="E6" s="3">
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1">
         <v>44317</v>
       </c>
       <c r="F6" s="1">
         <v>44319</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G6" s="1">
+        <v>44321</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44324</v>
+      </c>
+      <c r="I6" s="1">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1338</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="1">
         <v>44321</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44322</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44322</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44323</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
       <c r="B8">
         <v>1530</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>44335</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1542</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1559</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1581</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1584</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1627</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1634</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1650</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1695</v>
       </c>

</xml_diff>

<commit_message>
updating organizational sheet to reflect follow up e-mails, and removing files that were added accidentally
</commit_message>
<xml_diff>
--- a/documents/protocol_and_emails/organizationSheet.xlsx
+++ b/documents/protocol_and_emails/organizationSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EyegazeTrackerPINEntry\documents\protocol_and_emails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bflewis\Documents\EyegazeTrackerPINEntry\documents\protocol_and_emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E475C7-CEEB-4707-90EE-FBBE93D6E934}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10780DF8-327F-4184-8DBA-B7BFC096E8A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,22 +456,22 @@
   <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.89453125" customWidth="1"/>
+    <col min="2" max="2" width="15.20703125" customWidth="1"/>
+    <col min="3" max="3" width="19.5234375" customWidth="1"/>
+    <col min="4" max="4" width="23.41796875" customWidth="1"/>
+    <col min="5" max="5" width="12.20703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7890625" customWidth="1"/>
+    <col min="7" max="7" width="13.3125" customWidth="1"/>
+    <col min="8" max="11" width="9.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -555,7 +555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -587,7 +587,7 @@
         <v>44334</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -609,6 +609,12 @@
       <c r="G5" s="1">
         <v>44335</v>
       </c>
+      <c r="H5" s="1">
+        <v>44335</v>
+      </c>
+      <c r="I5" s="1">
+        <v>44386</v>
+      </c>
       <c r="K5" s="1">
         <v>44334</v>
       </c>
@@ -616,7 +622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -645,7 +651,7 @@
         <v>44335</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -677,7 +683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -690,973 +696,976 @@
       <c r="F8" s="1">
         <v>44335</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <v>44386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>1542</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>1559</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>1581</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>1584</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>1627</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>1634</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
         <v>1650</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>1695</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
         <v>1696</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18">
         <v>1719</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19">
         <v>1720</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
         <v>1770</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B21">
         <v>1809</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <v>1847</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
         <v>1877</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
         <v>2033</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
         <v>2047</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B26">
         <v>2065</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B27">
         <v>2112</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B28">
         <v>2165</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
         <v>2343</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B30">
         <v>2360</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B31">
         <v>2431</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B32">
         <v>2516</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B33">
         <v>2559</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B34">
         <v>2580</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B35">
         <v>2636</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B36">
         <v>2649</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B37">
         <v>2762</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B38">
         <v>2782</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B39">
         <v>2813</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B40">
         <v>2847</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B41">
         <v>2875</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B42">
         <v>2896</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B43">
         <v>2937</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B44">
         <v>2959</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B45">
         <v>3063</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B46">
         <v>3119</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B47">
         <v>3156</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B48">
         <v>3207</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B49">
         <v>3209</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B50">
         <v>3339</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B51">
         <v>3343</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B52">
         <v>3347</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B53">
         <v>3394</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B54">
         <v>3446</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B55">
         <v>3448</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B56">
         <v>3463</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B57">
         <v>3466</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B58">
         <v>3566</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B59">
         <v>3615</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B60">
         <v>3651</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B61">
         <v>3669</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B62">
         <v>3759</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B63">
         <v>3853</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B64">
         <v>3867</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B65">
         <v>3980</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B66">
         <v>4003</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B67">
         <v>4030</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B68">
         <v>4113</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B69">
         <v>4220</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B70">
         <v>4342</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B71">
         <v>4357</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B72">
         <v>4463</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B73">
         <v>4496</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B74">
         <v>4508</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B75">
         <v>4551</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B76">
         <v>4645</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B77">
         <v>4716</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B78">
         <v>4732</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B79">
         <v>4772</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B80">
         <v>4809</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B81">
         <v>4816</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B82">
         <v>4829</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B83">
         <v>4850</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B84">
         <v>4856</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B85">
         <v>4908</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B86">
         <v>4909</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B87">
         <v>4961</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B88">
         <v>5067</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B89">
         <v>5101</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B90">
         <v>5178</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B91">
         <v>5184</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B92">
         <v>5204</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B93">
         <v>5211</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B94">
         <v>5214</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B95">
         <v>5217</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B96">
         <v>5219</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B97">
         <v>5305</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B98">
         <v>5320</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B99">
         <v>5413</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B100">
         <v>5491</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B101">
         <v>5553</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B102">
         <v>5597</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B103">
         <v>5669</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B104">
         <v>5729</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B105">
         <v>5770</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B106">
         <v>5784</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B107">
         <v>5820</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B108">
         <v>5838</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B109">
         <v>5841</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B110">
         <v>5881</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B111">
         <v>5918</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B112">
         <v>5961</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B113">
         <v>5967</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B114">
         <v>6113</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B115">
         <v>6134</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B116">
         <v>6165</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B117">
         <v>6180</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B118">
         <v>6186</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B119">
         <v>6223</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B120">
         <v>6378</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B121">
         <v>6396</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B122">
         <v>6492</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B123">
         <v>6573</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B124">
         <v>6619</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B125">
         <v>6676</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B126">
         <v>6707</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B127">
         <v>6711</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B128">
         <v>6728</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B129">
         <v>6905</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B130">
         <v>6929</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B131">
         <v>6955</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B132">
         <v>6974</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B133">
         <v>7074</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B134">
         <v>7083</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B135">
         <v>7098</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B136">
         <v>7099</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B137">
         <v>7106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B138">
         <v>7113</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B139">
         <v>7147</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B140">
         <v>7153</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B141">
         <v>7155</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B142">
         <v>7157</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B143">
         <v>7232</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B144">
         <v>7262</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B145">
         <v>7270</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B146">
         <v>7281</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B147">
         <v>7347</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B148">
         <v>7399</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B149">
         <v>7409</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B150">
         <v>7433</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B151">
         <v>7481</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B152">
         <v>7597</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B153">
         <v>7610</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B154">
         <v>7620</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B155">
         <v>7701</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B156">
         <v>7846</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B157">
         <v>7852</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B158">
         <v>7941</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B159">
         <v>8050</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B160">
         <v>8238</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B161">
         <v>8244</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B162">
         <v>8266</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B163">
         <v>8287</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B164">
         <v>8346</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B165">
         <v>8438</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B166">
         <v>8470</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B167">
         <v>8496</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B168">
         <v>8505</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B169">
         <v>8598</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B170">
         <v>8678</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B171">
         <v>8681</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B172">
         <v>8758</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B173">
         <v>8772</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B174">
         <v>8819</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B175">
         <v>8896</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B176">
         <v>8901</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B177">
         <v>8918</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B178">
         <v>8952</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B179">
         <v>8965</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B180">
         <v>9018</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B181">
         <v>9059</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B182">
         <v>9095</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B183">
         <v>9144</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B184">
         <v>9147</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B185">
         <v>9176</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B186">
         <v>9181</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B187">
         <v>9192</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B188">
         <v>9207</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B189">
         <v>9214</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B190">
         <v>9281</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B191">
         <v>9324</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B192">
         <v>9349</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B193">
         <v>9352</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B194">
         <v>9372</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B195">
         <v>9505</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B196">
         <v>9546</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B197">
         <v>9568</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B198">
         <v>9692</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B199">
         <v>9759</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B200">
         <v>9767</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B201">
         <v>9850</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B202">
         <v>9914</v>
       </c>

</xml_diff>